<commit_message>
fixed bug in get_exposures; removed the need to define a schema beforehand
</commit_message>
<xml_diff>
--- a/tests/portfolio/reference_calculations.xlsx
+++ b/tests/portfolio/reference_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BenjaminYe\Projects\portana\tests\portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7CB547A-1851-49EC-B746-54711BF22BAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2983E5F1-A68E-42D5-9357-281E21EF23D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22305" yWindow="14340" windowWidth="29250" windowHeight="13935" xr2:uid="{E6AA1B9C-0A25-4E8F-8946-3E386F44CF91}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -130,7 +130,7 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C0F693-476D-4B30-8A63-6037C3C5AD99}">
   <dimension ref="B2:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +465,7 @@
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="5" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="10" width="14.7109375" customWidth="1"/>
+    <col min="8" max="11" width="14.7109375" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
   </cols>
@@ -514,6 +514,7 @@
       <c r="J5" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="K5" s="3"/>
       <c r="L5" s="4" t="s">
         <v>9</v>
       </c>
@@ -789,6 +790,7 @@
       <c r="J13" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="K13" s="3"/>
       <c r="L13" s="4" t="s">
         <v>9</v>
       </c>
@@ -822,15 +824,15 @@
         <v>43832</v>
       </c>
       <c r="H14">
-        <f>C21/SUM($C21:$E21)</f>
+        <f t="shared" ref="H14:J18" si="3">C21/SUM($C21:$E21)</f>
         <v>0.21351906828042935</v>
       </c>
       <c r="I14">
-        <f>D21/SUM($C21:$E21)</f>
+        <f t="shared" si="3"/>
         <v>0.27403516784654031</v>
       </c>
       <c r="J14">
-        <f>E21/SUM($C21:$E21)</f>
+        <f t="shared" si="3"/>
         <v>0.51244576387303042</v>
       </c>
       <c r="L14" s="1">
@@ -852,31 +854,31 @@
         <v>43833</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:E15" si="3">C8/C7-1</f>
+        <f t="shared" ref="C15:E15" si="4">C8/C7-1</f>
         <v>-4.705882352941182E-2</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15" si="4">D8/D7-1</f>
+        <f t="shared" ref="D15" si="5">D8/D7-1</f>
         <v>-2.5000000000000022E-2</v>
       </c>
       <c r="E15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.9215686274509887E-2</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" ref="G15:G18" si="5">G14+1</f>
+        <f t="shared" ref="G15:G18" si="6">G14+1</f>
         <v>43833</v>
       </c>
       <c r="H15">
-        <f>C22/SUM($C22:$E22)</f>
+        <f t="shared" si="3"/>
         <v>0.20282267243341681</v>
       </c>
       <c r="I15">
-        <f>D22/SUM($C22:$E22)</f>
+        <f t="shared" si="3"/>
         <v>0.26633280218529476</v>
       </c>
       <c r="J15">
-        <f>E22/SUM($C22:$E22)</f>
+        <f t="shared" si="3"/>
         <v>0.53084452538128846</v>
       </c>
       <c r="L15" s="1">
@@ -900,31 +902,31 @@
         <v>43834</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:E16" si="6">C9/C8-1</f>
+        <f t="shared" ref="C16:E16" si="7">C9/C8-1</f>
         <v>1.2345679012345734E-2</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="D16" si="7">D9/D8-1</f>
+        <f t="shared" ref="D16" si="8">D9/D8-1</f>
         <v>-0.10256410256410253</v>
       </c>
       <c r="E16">
+        <f t="shared" si="7"/>
+        <v>1.8867924528301883E-2</v>
+      </c>
+      <c r="G16" s="1">
         <f t="shared" si="6"/>
-        <v>1.8867924528301883E-2</v>
-      </c>
-      <c r="G16" s="1">
-        <f t="shared" si="5"/>
         <v>43834</v>
       </c>
       <c r="H16">
-        <f>C23/SUM($C23:$E23)</f>
+        <f t="shared" si="3"/>
         <v>0.20841035120147874</v>
       </c>
       <c r="I16">
-        <f>D23/SUM($C23:$E23)</f>
+        <f t="shared" si="3"/>
         <v>0.24260628465804066</v>
       </c>
       <c r="J16">
-        <f>E23/SUM($C23:$E23)</f>
+        <f t="shared" si="3"/>
         <v>0.54898336414048066</v>
       </c>
       <c r="L16" s="1">
@@ -935,11 +937,11 @@
         <v>-1.1951551881683575E-2</v>
       </c>
       <c r="O16" s="1">
-        <f t="shared" ref="O16:O19" si="8">O15+1</f>
+        <f t="shared" ref="O16:O19" si="9">O15+1</f>
         <v>43833</v>
       </c>
       <c r="P16">
-        <f t="shared" ref="P16:P19" si="9">P15*(1+M15)</f>
+        <f t="shared" ref="P16:P19" si="10">P15*(1+M15)</f>
         <v>100.32900011017676</v>
       </c>
     </row>
@@ -948,31 +950,31 @@
         <v>43835</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:E17" si="10">C10/C9-1</f>
+        <f t="shared" ref="C17:E17" si="11">C10/C9-1</f>
         <v>3.6585365853658569E-2</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D17" si="11">D10/D9-1</f>
+        <f t="shared" ref="D17" si="12">D10/D9-1</f>
         <v>-0.1428571428571429</v>
       </c>
       <c r="E17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.7037037037036979E-2</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43835</v>
       </c>
       <c r="H17">
-        <f>C24/SUM($C24:$E24)</f>
+        <f t="shared" si="3"/>
         <v>0.21749244010234942</v>
       </c>
       <c r="I17">
-        <f>D24/SUM($C24:$E24)</f>
+        <f t="shared" si="3"/>
         <v>0.209351011863224</v>
       </c>
       <c r="J17">
-        <f>E24/SUM($C24:$E24)</f>
+        <f t="shared" si="3"/>
         <v>0.57315654803442662</v>
       </c>
       <c r="L17" s="1">
@@ -983,11 +985,11 @@
         <v>-7.2222661991131268E-4</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>43834</v>
       </c>
       <c r="P17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>99.129912860122545</v>
       </c>
     </row>
@@ -996,31 +998,31 @@
         <v>43836</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:E18" si="12">C11/C10-1</f>
+        <f t="shared" ref="C18:E18" si="13">C11/C10-1</f>
         <v>5.8823529411764719E-2</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18" si="13">D11/D10-1</f>
+        <f t="shared" ref="D18" si="14">D11/D10-1</f>
         <v>6.6666666666666652E-2</v>
       </c>
       <c r="E18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-1.7857142857142905E-2</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43836</v>
       </c>
       <c r="H18">
-        <f>C25/SUM($C25:$E25)</f>
+        <f t="shared" si="3"/>
         <v>0.22654462242562931</v>
       </c>
       <c r="I18">
-        <f>D25/SUM($C25:$E25)</f>
+        <f t="shared" si="3"/>
         <v>0.21967963386727685</v>
       </c>
       <c r="J18">
-        <f>E25/SUM($C25:$E25)</f>
+        <f t="shared" si="3"/>
         <v>0.55377574370709381</v>
       </c>
       <c r="L18" s="1">
@@ -1031,21 +1033,21 @@
         <v>1.8082610618618128E-2</v>
       </c>
       <c r="O18" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>43835</v>
       </c>
       <c r="P18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>99.058318598225483</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="O19" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>43836</v>
       </c>
       <c r="P19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>100.84955160197221</v>
       </c>
     </row>
@@ -1087,15 +1089,15 @@
         <v>43833</v>
       </c>
       <c r="C22">
-        <f>C21*(1+C15)</f>
+        <f t="shared" ref="C22:E25" si="15">C21*(1+C15)</f>
         <v>0.20250000000000001</v>
       </c>
       <c r="D22">
-        <f>D21*(1+D15)</f>
+        <f t="shared" si="15"/>
         <v>0.26590909090909087</v>
       </c>
       <c r="E22">
-        <f>E21*(1+E15)</f>
+        <f t="shared" si="15"/>
         <v>0.53</v>
       </c>
     </row>
@@ -1105,15 +1107,15 @@
         <v>43834</v>
       </c>
       <c r="C23">
-        <f>C22*(1+C16)</f>
+        <f t="shared" si="15"/>
         <v>0.20500000000000002</v>
       </c>
       <c r="D23">
-        <f>D22*(1+D16)</f>
+        <f t="shared" si="15"/>
         <v>0.23863636363636362</v>
       </c>
       <c r="E23">
-        <f>E22*(1+E16)</f>
+        <f t="shared" si="15"/>
         <v>0.54</v>
       </c>
     </row>
@@ -1123,15 +1125,15 @@
         <v>43835</v>
       </c>
       <c r="C24">
-        <f>C23*(1+C17)</f>
+        <f t="shared" si="15"/>
         <v>0.21250000000000002</v>
       </c>
       <c r="D24">
-        <f>D23*(1+D17)</f>
+        <f t="shared" si="15"/>
         <v>0.20454545454545453</v>
       </c>
       <c r="E24">
-        <f>E23*(1+E17)</f>
+        <f t="shared" si="15"/>
         <v>0.56000000000000005</v>
       </c>
     </row>
@@ -1141,15 +1143,15 @@
         <v>43836</v>
       </c>
       <c r="C25">
-        <f>C24*(1+C18)</f>
+        <f t="shared" si="15"/>
         <v>0.22500000000000003</v>
       </c>
       <c r="D25">
-        <f>D24*(1+D18)</f>
+        <f t="shared" si="15"/>
         <v>0.21818181818181817</v>
       </c>
       <c r="E25">
-        <f>E24*(1+E18)</f>
+        <f t="shared" si="15"/>
         <v>0.55000000000000004</v>
       </c>
     </row>

</xml_diff>